<commit_message>
alteracao dfd e analise de eventos comprar produtos
</commit_message>
<xml_diff>
--- a/docs/ARTEFATOS(15-23)/COMPRAS/COMPRAR_PRODUTOS/Análise de Eventos_COMPRAR_PRODUTOS.xlsx
+++ b/docs/ARTEFATOS(15-23)/COMPRAS/COMPRAR_PRODUTOS/Análise de Eventos_COMPRAR_PRODUTOS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Externo</t>
   </si>
@@ -63,19 +63,22 @@
     <t xml:space="preserve">FB</t>
   </si>
   <si>
-    <t xml:space="preserve">O gerente realiza o orçamento</t>
+    <t xml:space="preserve">O cozinheiro entrega a lista de produtos em falta</t>
   </si>
   <si>
     <t xml:space="preserve">X</t>
   </si>
   <si>
-    <t xml:space="preserve">O gerente realiza a compra das mercadorias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O gerente verifica as mercadorias compradas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O gerente solicita a troca da mercadoria</t>
+    <t xml:space="preserve">O fornecedor envia o orçamento do pedido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O fornecedor entrega os produtos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X(2)</t>
   </si>
 </sst>
 </file>
@@ -204,7 +207,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -258,10 +261,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -344,15 +343,15 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4:G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="70"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.01"/>
@@ -436,7 +435,9 @@
       <c r="D4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="F4" s="9"/>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
@@ -450,31 +451,19 @@
         <v>3</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="9"/>
+        <v>17</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="F5" s="9"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
       <c r="J5" s="13"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="13"/>
-    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -482,8 +471,8 @@
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>